<commit_message>
Added result data for getTransitiveDistance.
</commit_message>
<xml_diff>
--- a/GraphSearching/result2.xlsx
+++ b/GraphSearching/result2.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="107" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="190" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -61,11 +61,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -83,11 +84,25 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Lohit Hindi"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -101,145 +116,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="medium"/>
       <diagonal/>
     </border>
   </borders>
@@ -267,14 +149,20 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -283,83 +171,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -371,10 +199,10 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Pivot Table Corner" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Pivot Table Value" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Pivot Table Field" xfId="22" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Pivot Table Category" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Pivot Table Corner" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Pivot Table Field" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Pivot Table Category" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Pivot Table Value" xfId="23" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -439,7 +267,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -473,7 +301,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -640,7 +468,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -807,7 +635,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -974,7 +802,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1116,11 +944,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="55558429"/>
-        <c:axId val="22407309"/>
+        <c:axId val="80193333"/>
+        <c:axId val="12469527"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55558429"/>
+        <c:axId val="80193333"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1145,7 +973,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>Number of Edges</a:t>
                 </a:r>
               </a:p>
@@ -1163,14 +991,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="22407309"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="12469527"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22407309"/>
+        <c:axId val="12469527"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,7 +1023,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>Time</a:t>
                 </a:r>
               </a:p>
@@ -1213,8 +1041,8 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="55558429"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="80193333"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1253,15 +1081,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>461880</xdr:colOff>
+      <xdr:colOff>489240</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>101880</xdr:rowOff>
+      <xdr:rowOff>93240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>181080</xdr:colOff>
+      <xdr:colOff>208080</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>50760</xdr:rowOff>
+      <xdr:rowOff>41400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1269,8 +1097,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4525560" y="264240"/>
-        <a:ext cx="7034400" cy="5150880"/>
+        <a:off x="4864680" y="255600"/>
+        <a:ext cx="7034040" cy="5150160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1283,15 +1111,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot1" cacheId="0" dataOnRows="false" dataPosition="65535" autoFormatId="1" dataCaption="Data" enableDrill="true" rowGrandTotals="false" colGrandTotals="false">
-  <location ref="A3:E23" firstHeaderRow="2" firstDataRow="4" firstDataCol="1" rowPageCount="19" colPageCount="4"/>
-  <rowFields count="1"/>
-  <colFields count="1"/>
-  <dataFields count="1"/>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -1300,7 +1119,7 @@
   <dimension ref="A1:F761"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -16552,12 +16371,13 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16572,358 +16392,358 @@
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="n">
-        <v>500</v>
-      </c>
-      <c r="B5" s="11" t="n">
+      <c r="A5" s="5" t="n">
+        <v>500</v>
+      </c>
+      <c r="B5" s="6" t="n">
         <v>129.7</v>
       </c>
-      <c r="C5" s="12" t="n">
+      <c r="C5" s="6" t="n">
         <v>2461.7</v>
       </c>
-      <c r="D5" s="12" t="n">
+      <c r="D5" s="6" t="n">
         <v>957.7</v>
       </c>
-      <c r="E5" s="13" t="n">
+      <c r="E5" s="6" t="n">
         <v>1892.3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="n">
+      <c r="A6" s="5" t="n">
         <v>1000</v>
       </c>
-      <c r="B6" s="15" t="n">
+      <c r="B6" s="6" t="n">
         <v>439.7</v>
       </c>
-      <c r="C6" s="16" t="n">
+      <c r="C6" s="6" t="n">
         <v>32689.8</v>
       </c>
-      <c r="D6" s="16" t="n">
+      <c r="D6" s="6" t="n">
         <v>8355.5</v>
       </c>
-      <c r="E6" s="17" t="n">
+      <c r="E6" s="6" t="n">
         <v>16284</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="n">
+      <c r="A7" s="5" t="n">
         <v>1500</v>
       </c>
-      <c r="B7" s="15" t="n">
+      <c r="B7" s="6" t="n">
         <v>346.8</v>
       </c>
-      <c r="C7" s="16" t="n">
+      <c r="C7" s="6" t="n">
         <v>45130.1</v>
       </c>
-      <c r="D7" s="16" t="n">
+      <c r="D7" s="6" t="n">
         <v>1446.8</v>
       </c>
-      <c r="E7" s="17" t="n">
+      <c r="E7" s="6" t="n">
         <v>28131.8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="n">
+      <c r="A8" s="5" t="n">
         <v>2000</v>
       </c>
-      <c r="B8" s="15" t="n">
+      <c r="B8" s="6" t="n">
         <v>138.1</v>
       </c>
-      <c r="C8" s="16" t="n">
+      <c r="C8" s="6" t="n">
         <v>19510.9</v>
       </c>
-      <c r="D8" s="16" t="n">
+      <c r="D8" s="6" t="n">
         <v>1458.3</v>
       </c>
-      <c r="E8" s="17" t="n">
+      <c r="E8" s="6" t="n">
         <v>30305.7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="n">
+      <c r="A9" s="5" t="n">
         <v>2500</v>
       </c>
-      <c r="B9" s="15" t="n">
+      <c r="B9" s="6" t="n">
         <v>121.1</v>
       </c>
-      <c r="C9" s="16" t="n">
+      <c r="C9" s="6" t="n">
         <v>14492.6</v>
       </c>
-      <c r="D9" s="16" t="n">
+      <c r="D9" s="6" t="n">
         <v>1638.1</v>
       </c>
-      <c r="E9" s="17" t="n">
+      <c r="E9" s="6" t="n">
         <v>17111.8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="n">
+      <c r="A10" s="5" t="n">
         <v>3000</v>
       </c>
-      <c r="B10" s="15" t="n">
+      <c r="B10" s="6" t="n">
         <v>115</v>
       </c>
-      <c r="C10" s="16" t="n">
+      <c r="C10" s="6" t="n">
         <v>21552.5</v>
       </c>
-      <c r="D10" s="16" t="n">
+      <c r="D10" s="6" t="n">
         <v>1540.8</v>
       </c>
-      <c r="E10" s="17" t="n">
+      <c r="E10" s="6" t="n">
         <v>14855</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="n">
+      <c r="A11" s="5" t="n">
         <v>3500</v>
       </c>
-      <c r="B11" s="15" t="n">
+      <c r="B11" s="6" t="n">
         <v>120.2</v>
       </c>
-      <c r="C11" s="16" t="n">
+      <c r="C11" s="6" t="n">
         <v>24118.7</v>
       </c>
-      <c r="D11" s="16" t="n">
+      <c r="D11" s="6" t="n">
         <v>1665.1</v>
       </c>
-      <c r="E11" s="17" t="n">
+      <c r="E11" s="6" t="n">
         <v>24136.7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="n">
+      <c r="A12" s="5" t="n">
         <v>4000</v>
       </c>
-      <c r="B12" s="15" t="n">
+      <c r="B12" s="6" t="n">
         <v>125.3</v>
       </c>
-      <c r="C12" s="16" t="n">
+      <c r="C12" s="6" t="n">
         <v>10495.3</v>
       </c>
-      <c r="D12" s="16" t="n">
+      <c r="D12" s="6" t="n">
         <v>1818.9</v>
       </c>
-      <c r="E12" s="17" t="n">
+      <c r="E12" s="6" t="n">
         <v>21791.1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="n">
+      <c r="A13" s="5" t="n">
         <v>4500</v>
       </c>
-      <c r="B13" s="15" t="n">
+      <c r="B13" s="6" t="n">
         <v>81.8</v>
       </c>
-      <c r="C13" s="16" t="n">
+      <c r="C13" s="6" t="n">
         <v>24064.6</v>
       </c>
-      <c r="D13" s="16" t="n">
+      <c r="D13" s="6" t="n">
         <v>1905.6</v>
       </c>
-      <c r="E13" s="17" t="n">
+      <c r="E13" s="6" t="n">
         <v>28623.2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="n">
+      <c r="A14" s="5" t="n">
         <v>5000</v>
       </c>
-      <c r="B14" s="15" t="n">
+      <c r="B14" s="6" t="n">
         <v>113.3</v>
       </c>
-      <c r="C14" s="16" t="n">
+      <c r="C14" s="6" t="n">
         <v>11221</v>
       </c>
-      <c r="D14" s="16" t="n">
+      <c r="D14" s="6" t="n">
         <v>1870</v>
       </c>
-      <c r="E14" s="17" t="n">
+      <c r="E14" s="6" t="n">
         <v>22946</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="n">
+      <c r="A15" s="5" t="n">
         <v>5500</v>
       </c>
-      <c r="B15" s="15" t="n">
+      <c r="B15" s="6" t="n">
         <v>119.8</v>
       </c>
-      <c r="C15" s="16" t="n">
+      <c r="C15" s="6" t="n">
         <v>27568.6</v>
       </c>
-      <c r="D15" s="16" t="n">
+      <c r="D15" s="6" t="n">
         <v>2020.3</v>
       </c>
-      <c r="E15" s="17" t="n">
+      <c r="E15" s="6" t="n">
         <v>30560.2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="n">
+      <c r="A16" s="5" t="n">
         <v>6000</v>
       </c>
-      <c r="B16" s="15" t="n">
+      <c r="B16" s="6" t="n">
         <v>109.6</v>
       </c>
-      <c r="C16" s="16" t="n">
+      <c r="C16" s="6" t="n">
         <v>29659.3</v>
       </c>
-      <c r="D16" s="16" t="n">
+      <c r="D16" s="6" t="n">
         <v>2002.5</v>
       </c>
-      <c r="E16" s="17" t="n">
+      <c r="E16" s="6" t="n">
         <v>24271.2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="n">
+      <c r="A17" s="5" t="n">
         <v>6500</v>
       </c>
-      <c r="B17" s="15" t="n">
+      <c r="B17" s="6" t="n">
         <v>120.6</v>
       </c>
-      <c r="C17" s="16" t="n">
+      <c r="C17" s="6" t="n">
         <v>21031.8</v>
       </c>
-      <c r="D17" s="16" t="n">
+      <c r="D17" s="6" t="n">
         <v>2112.2</v>
       </c>
-      <c r="E17" s="17" t="n">
+      <c r="E17" s="6" t="n">
         <v>73404.5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="n">
+      <c r="A18" s="5" t="n">
         <v>7000</v>
       </c>
-      <c r="B18" s="15" t="n">
+      <c r="B18" s="6" t="n">
         <v>181.6</v>
       </c>
-      <c r="C18" s="16" t="n">
+      <c r="C18" s="6" t="n">
         <v>16698.4</v>
       </c>
-      <c r="D18" s="16" t="n">
+      <c r="D18" s="6" t="n">
         <v>2290</v>
       </c>
-      <c r="E18" s="17" t="n">
+      <c r="E18" s="6" t="n">
         <v>13975.8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="n">
+      <c r="A19" s="5" t="n">
         <v>7500</v>
       </c>
-      <c r="B19" s="15" t="n">
+      <c r="B19" s="6" t="n">
         <v>170.8</v>
       </c>
-      <c r="C19" s="16" t="n">
+      <c r="C19" s="6" t="n">
         <v>23995.2</v>
       </c>
-      <c r="D19" s="16" t="n">
+      <c r="D19" s="6" t="n">
         <v>2606.7</v>
       </c>
-      <c r="E19" s="17" t="n">
+      <c r="E19" s="6" t="n">
         <v>22679.2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="n">
+      <c r="A20" s="5" t="n">
         <v>8000</v>
       </c>
-      <c r="B20" s="15" t="n">
+      <c r="B20" s="6" t="n">
         <v>144.4</v>
       </c>
-      <c r="C20" s="16" t="n">
+      <c r="C20" s="6" t="n">
         <v>18276</v>
       </c>
-      <c r="D20" s="16" t="n">
+      <c r="D20" s="6" t="n">
         <v>2492.9</v>
       </c>
-      <c r="E20" s="17" t="n">
+      <c r="E20" s="6" t="n">
         <v>23444.9</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="n">
+      <c r="A21" s="5" t="n">
         <v>8500</v>
       </c>
-      <c r="B21" s="15" t="n">
+      <c r="B21" s="6" t="n">
         <v>182.4</v>
       </c>
-      <c r="C21" s="16" t="n">
+      <c r="C21" s="6" t="n">
         <v>21431.3</v>
       </c>
-      <c r="D21" s="16" t="n">
+      <c r="D21" s="6" t="n">
         <v>2596</v>
       </c>
-      <c r="E21" s="17" t="n">
+      <c r="E21" s="6" t="n">
         <v>18886.9</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14" t="n">
+      <c r="A22" s="5" t="n">
         <v>9000</v>
       </c>
-      <c r="B22" s="15" t="n">
+      <c r="B22" s="6" t="n">
         <v>202.3</v>
       </c>
-      <c r="C22" s="16" t="n">
+      <c r="C22" s="6" t="n">
         <v>29944.5</v>
       </c>
-      <c r="D22" s="16" t="n">
+      <c r="D22" s="6" t="n">
         <v>2718.3</v>
       </c>
-      <c r="E22" s="17" t="n">
+      <c r="E22" s="6" t="n">
         <v>25231.2</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18" t="n">
+      <c r="A23" s="5" t="n">
         <v>9500</v>
       </c>
-      <c r="B23" s="19" t="n">
+      <c r="B23" s="6" t="n">
         <v>153.6</v>
       </c>
-      <c r="C23" s="20" t="n">
+      <c r="C23" s="6" t="n">
         <v>30347.1</v>
       </c>
-      <c r="D23" s="20" t="n">
+      <c r="D23" s="6" t="n">
         <v>2616.6</v>
       </c>
-      <c r="E23" s="21" t="n">
+      <c r="E23" s="6" t="n">
         <v>35732.6</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>